<commit_message>
can now read full range of integers with max precision
</commit_message>
<xml_diff>
--- a/Team Greybeards/Floating Point 2 Registers.xlsx
+++ b/Team Greybeards/Floating Point 2 Registers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="10515" windowHeight="4680"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>$s0</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Read First Char</t>
   </si>
   <si>
-    <t>0xf000</t>
-  </si>
-  <si>
     <t>UART Status bit</t>
   </si>
   <si>
@@ -114,37 +111,52 @@
     <t>Decimal Point Check</t>
   </si>
   <si>
-    <t># Digits to left of Decimal</t>
-  </si>
-  <si>
     <t>Constant 10</t>
   </si>
   <si>
     <t>0x30 (ascii to bin)</t>
   </si>
   <si>
-    <t>Read Digits</t>
-  </si>
-  <si>
     <t>nth character</t>
   </si>
   <si>
-    <t>0x0100 (Max mantissa)</t>
-  </si>
-  <si>
-    <t>Saved multiply result</t>
-  </si>
-  <si>
-    <t>max &lt; t8?</t>
-  </si>
-  <si>
-    <t>Read Digitsd No More Add</t>
-  </si>
-  <si>
-    <t>Constant 2</t>
-  </si>
-  <si>
-    <t>Read Digitsd No More Add Init</t>
+    <t>Read integers</t>
+  </si>
+  <si>
+    <t>0x7fffffff (data mask)</t>
+  </si>
+  <si>
+    <t>0xf0000000</t>
+  </si>
+  <si>
+    <t>1 in 32nd bit?</t>
+  </si>
+  <si>
+    <t>reg 1</t>
+  </si>
+  <si>
+    <t>reg 2</t>
+  </si>
+  <si>
+    <t>reg 3</t>
+  </si>
+  <si>
+    <t>reg 4</t>
+  </si>
+  <si>
+    <t>carry reg 1</t>
+  </si>
+  <si>
+    <t>carry reg 2</t>
+  </si>
+  <si>
+    <t>carry reg 3</t>
+  </si>
+  <si>
+    <t>saved register, w/o 32nd bit</t>
+  </si>
+  <si>
+    <t>nth_register</t>
   </si>
 </sst>
 </file>
@@ -491,22 +503,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I8" sqref="I8"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -514,25 +525,22 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -551,17 +559,11 @@
       <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -572,245 +574,200 @@
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
       <c r="G10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
       <c r="G12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begin working on numbers less than 1
</commit_message>
<xml_diff>
--- a/Team Greybeards/Floating Point 2 Registers.xlsx
+++ b/Team Greybeards/Floating Point 2 Registers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="10515" windowHeight="4680"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>$s0</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>nth_register</t>
+  </si>
+  <si>
+    <t>exponent</t>
+  </si>
+  <si>
+    <t>bits in register</t>
+  </si>
+  <si>
+    <t>result of shift</t>
+  </si>
+  <si>
+    <t>nth register mantissa check</t>
+  </si>
+  <si>
+    <t>more than 22 bits read in?</t>
+  </si>
+  <si>
+    <t>final mantissa</t>
   </si>
 </sst>
 </file>
@@ -503,11 +521,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,9 +533,11 @@
     <col min="2" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -539,8 +559,11 @@
       <c r="H1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -563,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -586,7 +609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -606,7 +629,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -626,7 +649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -649,12 +672,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -665,31 +691,40 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="G10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -703,7 +738,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -717,12 +752,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -730,7 +768,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>

</xml_diff>